<commit_message>
[MS-CPSWS] add 3 cases and 11 capture code for fixed TDIs\TDQs
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-CPSWS/MS-CPSWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-CPSWS/MS-CPSWS_RequirementSpecification.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$520</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$519</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3557" uniqueCount="1173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1171">
   <si>
     <t>Req ID</t>
   </si>
@@ -4197,12 +4197,6 @@
   </si>
   <si>
     <t>[In Search] If no provider names are specified, the protocol server MUST use all the available claims providers.&lt;5&gt;</t>
-  </si>
-  <si>
-    <t>MS-CPSWS_R381001</t>
-  </si>
-  <si>
-    <t>[In Search] For this operation[Search], the server will not use any available claims providers. [In Appendix B: Product Behavior](&lt;5&gt; Section 3.1.4.12: Windows SharePoint Services 3.0 and above follow this behavior)</t>
   </si>
   <si>
     <t>MS-CPSWS_R398001</t>
@@ -4486,6 +4480,21 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4510,100 +4519,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="33">
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4942,6 +4862,80 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5071,34 +5065,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I520" tableType="xml" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" connectionId="1">
-  <autoFilter ref="A19:I520"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I519" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I519"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="30">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="29">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="28">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="27">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="26">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="25">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="24">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="23">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="22">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -5107,12 +5101,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="16"/>
-    <tableColumn id="2" name="Test" dataDxfId="15"/>
-    <tableColumn id="3" name="Description" dataDxfId="14"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5440,11 +5434,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L522"/>
+  <dimension ref="A1:L521"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:I8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -5498,127 +5490,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -5631,12 +5623,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -5649,12 +5641,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -5667,12 +5659,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -5685,60 +5677,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -12220,7 +12212,7 @@
         <v>15</v>
       </c>
       <c r="H277" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I277" s="32"/>
     </row>
@@ -12245,7 +12237,7 @@
         <v>15</v>
       </c>
       <c r="H278" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I278" s="32"/>
     </row>
@@ -12895,7 +12887,7 @@
         <v>15</v>
       </c>
       <c r="H304" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I304" s="32"/>
     </row>
@@ -12920,7 +12912,7 @@
         <v>15</v>
       </c>
       <c r="H305" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I305" s="32"/>
     </row>
@@ -13495,7 +13487,7 @@
         <v>15</v>
       </c>
       <c r="H328" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I328" s="32"/>
     </row>
@@ -17026,13 +17018,13 @@
     </row>
     <row r="470" spans="1:9">
       <c r="A470" s="22" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B470" s="24" t="s">
         <v>643</v>
       </c>
       <c r="C470" s="20" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="D470" s="30"/>
       <c r="E470" s="30" t="s">
@@ -18001,13 +17993,13 @@
     </row>
     <row r="509" spans="1:9">
       <c r="A509" s="22" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="B509" s="24" t="s">
         <v>653</v>
       </c>
       <c r="C509" s="20" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="D509" s="22"/>
       <c r="E509" s="22" t="s">
@@ -18278,46 +18270,16 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="520" spans="1:9" ht="30">
-      <c r="A520" s="22" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B520" s="24" t="s">
-        <v>655</v>
-      </c>
-      <c r="C520" s="20" t="s">
-        <v>1168</v>
-      </c>
-      <c r="D520" s="30"/>
-      <c r="E520" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F520" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="G520" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H520" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I520" s="32"/>
+    <row r="520" spans="1:9">
+      <c r="A520" s="3"/>
+      <c r="B520" s="10"/>
     </row>
     <row r="521" spans="1:9">
       <c r="A521" s="3"/>
       <c r="B521" s="10"/>
     </row>
-    <row r="522" spans="1:9">
-      <c r="A522" s="3"/>
-      <c r="B522" s="10"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -18325,75 +18287,80 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:H275 I20:I453 A34:I469 A470:B470 D470:I470 A471:I520">
-    <cfRule type="expression" dxfId="13" priority="91">
+  <conditionalFormatting sqref="A20:H275 I20:I453 A34:I469 A470:B470 D470:I470 A471:I519">
+    <cfRule type="expression" dxfId="32" priority="91">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="92">
+    <cfRule type="expression" dxfId="31" priority="92">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="99">
+    <cfRule type="expression" dxfId="30" priority="99">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H275 I20:I453 A34:I469 A470:B470 D470:I470 A471:I520">
-    <cfRule type="expression" dxfId="10" priority="45">
+  <conditionalFormatting sqref="A20:H275 I20:I453 A34:I469 A470:B470 D470:I470 A471:I519">
+    <cfRule type="expression" dxfId="29" priority="45">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="46">
+    <cfRule type="expression" dxfId="28" priority="46">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="47">
+    <cfRule type="expression" dxfId="27" priority="47">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F520">
-    <cfRule type="expression" dxfId="7" priority="51">
+  <conditionalFormatting sqref="F20:F519">
+    <cfRule type="expression" dxfId="26" priority="51">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="52">
+    <cfRule type="expression" dxfId="25" priority="52">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C470">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C470">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F520">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F519">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E520">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E519">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G520">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G519">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H520">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H519">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -18403,7 +18370,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B521:B522 B19:B114 B116:B200 B202:B214 B216:B219 B221:B234 B236:B258 B260:B274 B276:B286 B510:B518 B288:B469 B471:B508" numberStoredAsText="1"/>
+    <ignoredError sqref="B519:B521 B19:B287 B509:B518 B288:B470 B471:B508 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -18422,12 +18389,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -18476,6 +18437,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
@@ -18485,20 +18452,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18511,4 +18464,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>